<commit_message>
Boxing website design finished
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB29B3-5623-42B1-85D6-A2EE9DEC28A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -258,11 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -543,11 +540,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,13 +621,13 @@
       <c r="J3" s="2"/>
       <c r="K3" s="13"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="19"/>
+      <c r="M3" s="15"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <v>2</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="13"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -640,7 +637,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="13"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="19"/>
+      <c r="M4" s="15"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
@@ -656,7 +653,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="19"/>
+      <c r="M5" s="15"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
@@ -672,7 +669,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="19"/>
+      <c r="M6" s="15"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
@@ -688,7 +685,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="19"/>
+      <c r="M7" s="15"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
@@ -696,7 +693,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="14"/>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="2"/>
@@ -712,7 +709,7 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="14"/>
+      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
@@ -728,7 +725,7 @@
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="14"/>
+      <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="2"/>
@@ -744,7 +741,7 @@
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="14"/>
+      <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
@@ -760,7 +757,7 @@
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="14"/>
+      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
@@ -862,7 +859,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="14"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="2"/>
       <c r="M18" s="7"/>
     </row>
@@ -878,7 +875,7 @@
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="14"/>
+      <c r="K19" s="1"/>
       <c r="L19" s="2"/>
       <c r="M19" s="7"/>
     </row>
@@ -894,7 +891,7 @@
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="14"/>
+      <c r="K20" s="1"/>
       <c r="L20" s="2"/>
       <c r="M20" s="7"/>
     </row>
@@ -910,7 +907,7 @@
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="14"/>
+      <c r="K21" s="1"/>
       <c r="L21" s="2"/>
       <c r="M21" s="7"/>
     </row>
@@ -926,23 +923,9 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="15"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="14"/>
       <c r="M22" s="10"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="16"/>
-      <c r="M23" s="16"/>
     </row>
     <row r="27" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>